<commit_message>
updated 4 january 2025
</commit_message>
<xml_diff>
--- a/Dataset/unique_pallete.xlsx
+++ b/Dataset/unique_pallete.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -888,6 +888,34 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>MF49C0012</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>MF49F0062</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>MF4970266</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>MF49G0263</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>